<commit_message>
Adding recent spreadsheet data to excel
</commit_message>
<xml_diff>
--- a/docs/exoskeleton_first_measurements.xlsx
+++ b/docs/exoskeleton_first_measurements.xlsx
@@ -291,7 +291,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -666,7 +665,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -773,7 +771,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1256,7 +1253,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3141,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added components list to repo
</commit_message>
<xml_diff>
--- a/docs/exoskeleton_first_measurements.xlsx
+++ b/docs/exoskeleton_first_measurements.xlsx
@@ -3152,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="E3" s="2">
         <f>(K10/A3)</f>
-        <v>1980</v>
+        <v>1204.5</v>
       </c>
       <c r="J3" s="5">
         <v>140</v>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="E4" s="2">
         <f>(K10/A4)</f>
-        <v>990</v>
+        <v>602.25</v>
       </c>
       <c r="J4" s="5">
         <v>5</v>
@@ -3284,7 +3284,7 @@
       </c>
       <c r="E5" s="2">
         <f>(K10/A5)</f>
-        <v>660</v>
+        <v>401.5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="E6" s="2">
         <f>(K10/A6)</f>
-        <v>495</v>
+        <v>301.125</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="E7" s="2">
         <f>(K10/A7)</f>
-        <v>396</v>
+        <v>240.89999999999998</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -3339,31 +3339,31 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>0.06</v>
+        <v>3.6499999999999998E-2</v>
       </c>
       <c r="B8" s="4">
         <v>80</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>8.3733333333333326E-2</v>
+        <v>5.0937777777777769E-2</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>0.33493333333333331</v>
+        <v>0.20375111111111108</v>
       </c>
       <c r="E8" s="4">
         <f>(K10/A8)</f>
         <v>330</v>
       </c>
       <c r="K8">
-        <v>0.06</v>
+        <v>3.6499999999999998E-2</v>
       </c>
       <c r="L8">
         <v>0.05</v>
       </c>
       <c r="M8">
-        <v>0.03</v>
+        <v>1.6250000000000001E-2</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>18</v>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="E9" s="2">
         <f>(K10/A9)</f>
-        <v>282.85714285714283</v>
+        <v>172.07142857142856</v>
       </c>
       <c r="K9">
         <v>330</v>
@@ -3418,11 +3418,11 @@
       </c>
       <c r="E10" s="2">
         <f>(K10/A10)</f>
-        <v>247.5</v>
+        <v>150.5625</v>
       </c>
       <c r="K10">
         <f>PRODUCT(K8,K9)</f>
-        <v>19.8</v>
+        <v>12.045</v>
       </c>
       <c r="L10">
         <f>PRODUCT(L8,L9)</f>
@@ -3430,7 +3430,7 @@
       </c>
       <c r="M10">
         <f>PRODUCT(M8,M9)</f>
-        <v>7.08</v>
+        <v>3.835</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>20</v>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="E11" s="2">
         <f>(K10/A11)</f>
-        <v>220.00000000000003</v>
+        <v>133.83333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="E12" s="2">
         <f>(K10/A12)</f>
-        <v>198</v>
+        <v>120.44999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="E13" s="2">
         <f>(K10/A13)</f>
-        <v>180</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="E14" s="2">
         <f>(K10/A14)</f>
-        <v>165</v>
+        <v>100.375</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="E15" s="2">
         <f>(K10/A15)</f>
-        <v>152.30769230769232</v>
+        <v>92.653846153846146</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="E16" s="2">
         <f>(K10/A16)</f>
-        <v>141.42857142857142</v>
+        <v>86.035714285714278</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="E17" s="2">
         <f>(K10/A17)</f>
-        <v>132</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="E18" s="2">
         <f>(K10/A18)</f>
-        <v>123.75</v>
+        <v>75.28125</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="E19" s="2">
         <f>(K10/A19)</f>
-        <v>116.47058823529412</v>
+        <v>70.85294117647058</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="E20" s="2">
         <f>(K10/A20)</f>
-        <v>110.00000000000001</v>
+        <v>66.916666666666671</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="E49" s="2">
         <f>(M10/A49)</f>
-        <v>1416</v>
+        <v>767</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="E50" s="2">
         <f>(M10/A50)</f>
-        <v>708</v>
+        <v>383.5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="E51" s="2">
         <f>(M10/A51)</f>
-        <v>472</v>
+        <v>255.66666666666669</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="E52" s="2">
         <f>(M10/A52)</f>
-        <v>354</v>
+        <v>191.75</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4155,23 +4155,23 @@
       </c>
       <c r="E53" s="2">
         <f>(M10/A53)</f>
-        <v>283.2</v>
+        <v>153.39999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
-        <v>0.03</v>
+        <v>1.6250000000000001E-2</v>
       </c>
       <c r="B54" s="4">
         <v>95</v>
       </c>
       <c r="C54" s="4">
         <f>(B54/360)*2*3.14*A54</f>
-        <v>4.9716666666666666E-2</v>
+        <v>2.6929861111111116E-2</v>
       </c>
       <c r="D54" s="4">
         <f>(C54*K4)</f>
-        <v>0.24858333333333332</v>
+        <v>0.13464930555555557</v>
       </c>
       <c r="E54" s="4">
         <f>(M10/A54)</f>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="E55" s="2">
         <f>(M10/A55)</f>
-        <v>202.28571428571428</v>
+        <v>109.57142857142856</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="E56" s="2">
         <f>(M10/A56)</f>
-        <v>177</v>
+        <v>95.875</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="E57" s="2">
         <f>(M10/A57)</f>
-        <v>157.33333333333334</v>
+        <v>85.222222222222229</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="E58" s="2">
         <f>(M10/A58)</f>
-        <v>141.6</v>
+        <v>76.699999999999989</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4275,7 +4275,7 @@
       </c>
       <c r="E59" s="2">
         <f>(M10/A59)</f>
-        <v>128.72727272727272</v>
+        <v>69.72727272727272</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="E60" s="2">
         <f>(M10/A60)</f>
-        <v>118</v>
+        <v>63.916666666666671</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="E61" s="2">
         <f>(M10/A61)</f>
-        <v>108.92307692307692</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="E62" s="2">
         <f>(M10/A62)</f>
-        <v>101.14285714285714</v>
+        <v>54.785714285714278</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4355,7 +4355,7 @@
       </c>
       <c r="E63" s="2">
         <f>(M10/A63)</f>
-        <v>94.4</v>
+        <v>51.133333333333333</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="E64" s="2">
         <f>(M10/A64)</f>
-        <v>88.5</v>
+        <v>47.9375</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E65" s="2">
         <f>(M10/A65)</f>
-        <v>83.294117647058812</v>
+        <v>45.117647058823529</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -4415,7 +4415,7 @@
       </c>
       <c r="E66" s="2">
         <f>(M10/A66)</f>
-        <v>78.666666666666671</v>
+        <v>42.611111111111114</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>